<commit_message>
dayle update 28 march
</commit_message>
<xml_diff>
--- a/Areas_salud.xlsx
+++ b/Areas_salud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javiercanalesluna/Desktop/Documentos/repositories/covid19_extremadura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1A81D-9A54-2041-9668-B9A778331257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A5A61D-B6E8-6A46-9F41-580D18F29425}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8D5962D6-3F8F-0F4F-BB97-4C14EAB963CA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{8D5962D6-3F8F-0F4F-BB97-4C14EAB963CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>